<commit_message>
dynamic Prdocut Search and Click
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\DataForDynamicTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\repository\Temp\Selenium-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C14582-D9F8-4E75-A01F-9681C031E454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B7AD02-9852-405C-B539-7360C52CB1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="960" windowWidth="14370" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
     <t>admin</t>
   </si>
   <si>
-    <t>POLO</t>
+    <t>Beanie</t>
   </si>
 </sst>
 </file>
@@ -372,19 +373,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C20BC6D-42D2-4785-8735-DC09237E1BA5}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD6613A-EB18-4D53-B3A5-E9C23E9E5E54}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>20</v>
       </c>
     </row>

</xml_diff>